<commit_message>
Market and Contract pricing
Addition of Market and Contract pricing model
</commit_message>
<xml_diff>
--- a/Hydropower_Fluctuations (2018).xlsx
+++ b/Hydropower_Fluctuations (2018).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Class project\GCD_BugFlowExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C661295-A439-4BEB-8291-0416D2D79AA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47C6667-7660-432B-939E-3788D95B953F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" xr2:uid="{A81DFEFB-5B04-4B3A-93E1-B49457620F3E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="28">
   <si>
     <t>Min Power</t>
   </si>
@@ -169,14 +169,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2482B0D3-E720-4E26-844E-49B7B4BAF006}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -504,34 +504,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>43160</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -648,19 +648,19 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>43191</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
@@ -777,19 +777,19 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <v>43221</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
@@ -906,19 +906,19 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="2">
+      <c r="A24" s="3">
         <v>43252</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
@@ -1035,19 +1035,19 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="2">
+      <c r="A31" s="3">
         <v>43282</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
@@ -1164,19 +1164,19 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="2">
+      <c r="A38" s="3">
         <v>43313</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
@@ -1293,19 +1293,19 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="2">
+      <c r="A45" s="3">
         <v>43344</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
@@ -1422,19 +1422,19 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="2">
+      <c r="A52" s="3">
         <v>43374</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">

</xml_diff>